<commit_message>
Agregué recopilacion de datos, falta agregar gráficas y conclusion
</commit_message>
<xml_diff>
--- a/Estadísticas.xlsx
+++ b/Estadísticas.xlsx
@@ -85,10 +85,10 @@
     <t>c.3.1) Intervalo = 10; CPU's = 2</t>
   </si>
   <si>
-    <t>c.3.3) Intervalo = 10; CPU's = 2</t>
+    <t>c.3.2) Intervalo = 5; CPU's = 2</t>
   </si>
   <si>
-    <t>c.3.2) Intervalo = 10; CPU's = 2</t>
+    <t>c.3.3) Intervalo = 1; CPU's = 2</t>
   </si>
 </sst>
 </file>
@@ -193,6 +193,1392 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Tiempo contra procesos: Tiempo</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> promedio de los procesos en la computadora con configuración normal</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>t</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="7.4700349956255463E-2"/>
+                  <c:y val="0.17183625730994151"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-GT"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$A$3:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$3:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>13.76</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.83</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23.14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-7578-4FE2-97E0-8D15AC03AD6D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="370593832"/>
+        <c:axId val="370596784"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="370593832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-GT"/>
+                  <a:t>Numero de procesos (n)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-GT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="370596784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="370596784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-GT"/>
+                  <a:t>Tiempo promedio (t)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-GT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="370593832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-GT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Tiempo contra procesos: Tiempo</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> promedio de los procesos en la computadora con configuración normal e intervalo 5</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>t</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="7.4700349956255463E-2"/>
+                  <c:y val="0.17183625730994151"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-GT"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$A$18:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$18:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>32.04</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>56.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128.76</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>209.24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300.60000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3657-45E6-BDB3-51E25210F6E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="370593832"/>
+        <c:axId val="370596784"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="370593832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-GT"/>
+                  <a:t>Numero de procesos (n)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-GT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="370596784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="370596784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-GT"/>
+                  <a:t>Tiempo promedio (t)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-GT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="370593832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-GT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Tiempo contra procesos: Tiempo</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> promedio de los procesos en la computadora con configuración normal e intervalo 1</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>t</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="7.4700349956255463E-2"/>
+                  <c:y val="0.17183625730994151"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-GT"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$A$33:$A$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$33:$B$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>98.16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>159.13999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>368.64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>517.73</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>673.53</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B16E-414B-8557-10C7E2C107CB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="370593832"/>
+        <c:axId val="370596784"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="370593832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-GT"/>
+                  <a:t>Numero de procesos (n)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-GT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="370596784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="370596784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-GT"/>
+                  <a:t>Tiempo promedio (t)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-GT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="370593832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-GT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Gráfico 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Gráfico 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -492,10 +1878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C106"/>
+  <dimension ref="A1:C124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -576,257 +1962,245 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
     <row r="10" spans="1:3">
-      <c r="A10" t="s">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="2" t="s">
+    <row r="17" spans="1:3">
+      <c r="A17" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="1">
+    <row r="18" spans="1:3">
+      <c r="A18" s="1">
         <v>25</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B18" s="4">
         <v>32.04</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C18" s="4">
         <v>27.71</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="1">
+    <row r="19" spans="1:3">
+      <c r="A19" s="1">
         <v>50</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B19" s="4">
         <v>56.7</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C19" s="4">
         <v>39.9</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1">
+    <row r="20" spans="1:3">
+      <c r="A20" s="1">
         <v>100</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B20" s="4">
         <v>128.76</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C20" s="4">
         <v>83.82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="1">
-        <v>150</v>
-      </c>
-      <c r="B15" s="4">
-        <v>209.24</v>
-      </c>
-      <c r="C15" s="4">
-        <v>133.29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="1">
-        <v>200</v>
-      </c>
-      <c r="B16" s="4">
-        <v>300.60000000000002</v>
-      </c>
-      <c r="C16" s="4">
-        <v>194.64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1">
-        <v>25</v>
+        <v>150</v>
       </c>
       <c r="B21" s="4">
-        <v>98.16</v>
+        <v>209.24</v>
       </c>
       <c r="C21" s="4">
-        <v>43.19</v>
+        <v>133.29</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="B22" s="4">
-        <v>159.13999999999999</v>
+        <v>300.60000000000002</v>
       </c>
       <c r="C22" s="4">
-        <v>78.56</v>
+        <v>194.64</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="1">
-        <v>100</v>
-      </c>
-      <c r="B23" s="4">
-        <v>368.64</v>
-      </c>
-      <c r="C23" s="4">
-        <v>190.52</v>
-      </c>
+      <c r="A23" s="1"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="1">
-        <v>150</v>
-      </c>
-      <c r="B24" s="4">
-        <v>517.73</v>
-      </c>
-      <c r="C24" s="4">
-        <v>277.88</v>
-      </c>
+      <c r="A24" s="1"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="1">
-        <v>200</v>
-      </c>
-      <c r="B25" s="4">
-        <v>673.53</v>
-      </c>
-      <c r="C25" s="4">
-        <v>378.11</v>
-      </c>
+      <c r="A25" s="1"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>6</v>
-      </c>
+      <c r="A28" s="1"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="2" t="s">
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="1">
-        <v>25</v>
-      </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="1">
-        <v>50</v>
-      </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="1">
-        <v>100</v>
-      </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="1">
-        <v>150</v>
-      </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
+        <v>25</v>
+      </c>
+      <c r="B33" s="4">
+        <v>98.16</v>
+      </c>
+      <c r="C33" s="4">
+        <v>43.19</v>
+      </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1">
+        <v>50</v>
+      </c>
+      <c r="B34" s="4">
+        <v>159.13999999999999</v>
+      </c>
+      <c r="C34" s="4">
+        <v>78.56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="1">
+        <v>100</v>
+      </c>
+      <c r="B35" s="4">
+        <v>368.64</v>
+      </c>
+      <c r="C35" s="4">
+        <v>190.52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="1">
+        <v>150</v>
+      </c>
+      <c r="B36" s="4">
+        <v>517.73</v>
+      </c>
+      <c r="C36" s="4">
+        <v>277.88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="1">
         <v>200</v>
       </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
-        <v>7</v>
+      <c r="B37" s="4">
+        <v>673.53</v>
+      </c>
+      <c r="C37" s="4">
+        <v>378.11</v>
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="A38" s="1"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="1">
-        <v>25</v>
-      </c>
+      <c r="A39" s="1"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="1">
-        <v>50</v>
-      </c>
+      <c r="A40" s="1"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="1">
-        <v>100</v>
-      </c>
+      <c r="A41" s="1"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="1">
-        <v>150</v>
-      </c>
+      <c r="A42" s="1"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="1">
-        <v>200</v>
-      </c>
+      <c r="A43" s="1"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -844,40 +2218,60 @@
       <c r="A48" s="1">
         <v>25</v>
       </c>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
+      <c r="B48" s="4">
+        <v>13.76</v>
+      </c>
+      <c r="C48" s="4">
+        <v>9.07</v>
+      </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="1">
         <v>50</v>
       </c>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
+      <c r="B49" s="4">
+        <v>14.44</v>
+      </c>
+      <c r="C49" s="4">
+        <v>9.08</v>
+      </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="1">
         <v>100</v>
       </c>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
+      <c r="B50" s="4">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="C50" s="4">
+        <v>13.49</v>
+      </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="1">
         <v>150</v>
       </c>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
+      <c r="B51" s="4">
+        <v>20.83</v>
+      </c>
+      <c r="C51" s="4">
+        <v>13.82</v>
+      </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="1">
         <v>200</v>
       </c>
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
+      <c r="B52" s="4">
+        <v>23.14</v>
+      </c>
+      <c r="C52" s="4">
+        <v>15.5</v>
+      </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -895,40 +2289,60 @@
       <c r="A57" s="1">
         <v>25</v>
       </c>
-      <c r="B57" s="4"/>
-      <c r="C57" s="4"/>
+      <c r="B57" s="4">
+        <v>32.04</v>
+      </c>
+      <c r="C57" s="4">
+        <v>27.71</v>
+      </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="1">
         <v>50</v>
       </c>
-      <c r="B58" s="4"/>
-      <c r="C58" s="4"/>
+      <c r="B58" s="4">
+        <v>56.7</v>
+      </c>
+      <c r="C58" s="4">
+        <v>39.9</v>
+      </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="1">
         <v>100</v>
       </c>
-      <c r="B59" s="4"/>
-      <c r="C59" s="4"/>
+      <c r="B59" s="4">
+        <v>143.02000000000001</v>
+      </c>
+      <c r="C59" s="4">
+        <v>112.25</v>
+      </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="1">
         <v>150</v>
       </c>
-      <c r="B60" s="4"/>
-      <c r="C60" s="4"/>
+      <c r="B60" s="4">
+        <v>207.76</v>
+      </c>
+      <c r="C60" s="4">
+        <v>139.19</v>
+      </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="1">
         <v>200</v>
       </c>
-      <c r="B61" s="4"/>
-      <c r="C61" s="4"/>
+      <c r="B61" s="4">
+        <v>261.35000000000002</v>
+      </c>
+      <c r="C61" s="4">
+        <v>158.94</v>
+      </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -946,42 +2360,61 @@
       <c r="A66" s="1">
         <v>25</v>
       </c>
-      <c r="B66" s="4"/>
-      <c r="C66" s="4"/>
+      <c r="B66" s="4">
+        <v>110.48</v>
+      </c>
+      <c r="C66" s="4">
+        <v>52.13</v>
+      </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="1">
         <v>50</v>
       </c>
-      <c r="B67" s="4"/>
-      <c r="C67" s="4"/>
+      <c r="B67" s="4">
+        <v>184.02</v>
+      </c>
+      <c r="C67" s="4">
+        <v>92.29</v>
+      </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="1">
         <v>100</v>
       </c>
-      <c r="B68" s="4"/>
-      <c r="C68" s="4"/>
+      <c r="B68" s="4">
+        <v>395.36</v>
+      </c>
+      <c r="C68" s="4">
+        <v>197.75</v>
+      </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="1">
         <v>150</v>
       </c>
-      <c r="B69" s="4"/>
-      <c r="C69" s="4"/>
+      <c r="B69" s="4">
+        <v>511.07</v>
+      </c>
+      <c r="C69" s="4">
+        <v>254.66</v>
+      </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="1">
         <v>200</v>
       </c>
-      <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
+      <c r="B70" s="4">
+        <v>700.59</v>
+      </c>
+      <c r="C70" s="4">
+        <v>368.3</v>
+      </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>11</v>
-      </c>
-      <c r="C73" s="5"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="2" t="s">
@@ -998,42 +2431,61 @@
       <c r="A75" s="1">
         <v>25</v>
       </c>
-      <c r="B75" s="4"/>
-      <c r="C75" s="4"/>
+      <c r="B75" s="4">
+        <v>8.44</v>
+      </c>
+      <c r="C75" s="4">
+        <v>5.1100000000000003</v>
+      </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="1">
         <v>50</v>
       </c>
-      <c r="B76" s="4"/>
-      <c r="C76" s="4"/>
+      <c r="B76" s="4">
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="C76" s="4">
+        <v>7.15</v>
+      </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="1">
         <v>100</v>
       </c>
-      <c r="B77" s="4"/>
-      <c r="C77" s="4"/>
+      <c r="B77" s="4">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="C77" s="4">
+        <v>7.07</v>
+      </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="1">
         <v>150</v>
       </c>
-      <c r="B78" s="4"/>
-      <c r="C78" s="4"/>
+      <c r="B78" s="4">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="C78" s="4">
+        <v>7.64</v>
+      </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="1">
         <v>200</v>
       </c>
-      <c r="B79" s="4"/>
-      <c r="C79" s="4"/>
+      <c r="B79" s="4">
+        <v>8.86</v>
+      </c>
+      <c r="C79" s="4">
+        <v>7.17</v>
+      </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>12</v>
-      </c>
-      <c r="C82" s="5"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="2" t="s">
@@ -1050,40 +2502,60 @@
       <c r="A84" s="1">
         <v>25</v>
       </c>
-      <c r="B84" s="4"/>
-      <c r="C84" s="4"/>
+      <c r="B84" s="4">
+        <v>12.68</v>
+      </c>
+      <c r="C84" s="4">
+        <v>9.06</v>
+      </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="1">
         <v>50</v>
       </c>
-      <c r="B85" s="4"/>
-      <c r="C85" s="4"/>
+      <c r="B85" s="4">
+        <v>10.36</v>
+      </c>
+      <c r="C85" s="4">
+        <v>7.96</v>
+      </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="1">
         <v>100</v>
       </c>
-      <c r="B86" s="4"/>
-      <c r="C86" s="4"/>
+      <c r="B86" s="4">
+        <v>32.479999999999997</v>
+      </c>
+      <c r="C86" s="4">
+        <v>33.22</v>
+      </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" s="1">
         <v>150</v>
       </c>
-      <c r="B87" s="4"/>
-      <c r="C87" s="4"/>
+      <c r="B87" s="4">
+        <v>40.65</v>
+      </c>
+      <c r="C87" s="4">
+        <v>32.21</v>
+      </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" s="1">
         <v>200</v>
       </c>
-      <c r="B88" s="4"/>
-      <c r="C88" s="4"/>
+      <c r="B88" s="4">
+        <v>38.93</v>
+      </c>
+      <c r="C88" s="4">
+        <v>29.77</v>
+      </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C91" s="5"/>
     </row>
@@ -1102,40 +2574,60 @@
       <c r="A93" s="1">
         <v>25</v>
       </c>
-      <c r="B93" s="4"/>
-      <c r="C93" s="4"/>
+      <c r="B93" s="4">
+        <v>57.84</v>
+      </c>
+      <c r="C93" s="4">
+        <v>27.14</v>
+      </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" s="1">
         <v>50</v>
       </c>
-      <c r="B94" s="4"/>
-      <c r="C94" s="4"/>
+      <c r="B94" s="4">
+        <v>106.74</v>
+      </c>
+      <c r="C94" s="4">
+        <v>49.26</v>
+      </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" s="1">
         <v>100</v>
       </c>
-      <c r="B95" s="4"/>
-      <c r="C95" s="4"/>
+      <c r="B95" s="4">
+        <v>208.32</v>
+      </c>
+      <c r="C95" s="4">
+        <v>117.15</v>
+      </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="1">
         <v>150</v>
       </c>
-      <c r="B96" s="4"/>
-      <c r="C96" s="4"/>
+      <c r="B96" s="4">
+        <v>288.04000000000002</v>
+      </c>
+      <c r="C96" s="4">
+        <v>174.35</v>
+      </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" s="1">
         <v>200</v>
       </c>
-      <c r="B97" s="4"/>
-      <c r="C97" s="4"/>
+      <c r="B97" s="4">
+        <v>346.57</v>
+      </c>
+      <c r="C97" s="4">
+        <v>203.31</v>
+      </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C100" s="5"/>
     </row>
@@ -1154,39 +2646,204 @@
       <c r="A102" s="1">
         <v>25</v>
       </c>
-      <c r="B102" s="4"/>
-      <c r="C102" s="4"/>
+      <c r="B102" s="4">
+        <v>10.88</v>
+      </c>
+      <c r="C102" s="4">
+        <v>6.45</v>
+      </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" s="1">
         <v>50</v>
       </c>
-      <c r="B103" s="4"/>
-      <c r="C103" s="4"/>
+      <c r="B103" s="4">
+        <v>8.98</v>
+      </c>
+      <c r="C103" s="4">
+        <v>6.32</v>
+      </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" s="1">
         <v>100</v>
       </c>
-      <c r="B104" s="4"/>
-      <c r="C104" s="4"/>
+      <c r="B104" s="4">
+        <v>8.77</v>
+      </c>
+      <c r="C104" s="4">
+        <v>6.12</v>
+      </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" s="1">
         <v>150</v>
       </c>
-      <c r="B105" s="4"/>
-      <c r="C105" s="4"/>
+      <c r="B105" s="4">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="C105" s="4">
+        <v>6.11</v>
+      </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" s="1">
         <v>200</v>
       </c>
-      <c r="B106" s="4"/>
-      <c r="C106" s="4"/>
+      <c r="B106" s="4">
+        <v>8.5250000000000004</v>
+      </c>
+      <c r="C106" s="4">
+        <v>6.06</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" t="s">
+        <v>13</v>
+      </c>
+      <c r="C109" s="5"/>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" s="1">
+        <v>25</v>
+      </c>
+      <c r="B111" s="4">
+        <v>9.36</v>
+      </c>
+      <c r="C111" s="4">
+        <v>7.89</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" s="1">
+        <v>50</v>
+      </c>
+      <c r="B112" s="4">
+        <v>17.72</v>
+      </c>
+      <c r="C112" s="4">
+        <v>17.38</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" s="1">
+        <v>100</v>
+      </c>
+      <c r="B113" s="4">
+        <v>27.28</v>
+      </c>
+      <c r="C113" s="4">
+        <v>23.75</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" s="1">
+        <v>150</v>
+      </c>
+      <c r="B114" s="4">
+        <v>23.11</v>
+      </c>
+      <c r="C114" s="4">
+        <v>21.46</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" s="1">
+        <v>200</v>
+      </c>
+      <c r="B115" s="4">
+        <v>20.13</v>
+      </c>
+      <c r="C115" s="4">
+        <v>19.61</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" t="s">
+        <v>14</v>
+      </c>
+      <c r="C118" s="5"/>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" s="1">
+        <v>25</v>
+      </c>
+      <c r="B120" s="4">
+        <v>44.32</v>
+      </c>
+      <c r="C120" s="4">
+        <v>24.93</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" s="1">
+        <v>50</v>
+      </c>
+      <c r="B121" s="4">
+        <v>78.12</v>
+      </c>
+      <c r="C121" s="4">
+        <v>41.37</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="1">
+        <v>100</v>
+      </c>
+      <c r="B122" s="4">
+        <v>152.9</v>
+      </c>
+      <c r="C122" s="4">
+        <v>93.39</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" s="1">
+        <v>150</v>
+      </c>
+      <c r="B123" s="4">
+        <v>214.37</v>
+      </c>
+      <c r="C123" s="4">
+        <v>124.79</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" s="1">
+        <v>200</v>
+      </c>
+      <c r="B124" s="4">
+        <v>272.02</v>
+      </c>
+      <c r="C124" s="4">
+        <v>149.24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>